<commit_message>
update requirments and resume
</commit_message>
<xml_diff>
--- a/Week12. second_turn_start/Resume12.xlsx
+++ b/Week12. second_turn_start/Resume12.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
   <si>
     <t>Фамилия</t>
   </si>
@@ -109,10 +109,10 @@
     <t>Реализация возможности проверки задачи и вынесения вердикта</t>
   </si>
   <si>
-    <t>,</t>
-  </si>
-  <si>
     <t>Асеев, Руданов</t>
+  </si>
+  <si>
+    <t>Макет страницы выбранной задачи</t>
   </si>
 </sst>
 </file>
@@ -467,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,7 +513,9 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="4"/>
+      <c r="D2" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
@@ -525,7 +527,9 @@
       <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="4"/>
+      <c r="D3" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
@@ -537,7 +541,9 @@
       <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="4"/>
+      <c r="D4" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
@@ -549,7 +555,9 @@
       <c r="C5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="4"/>
+      <c r="D5" s="4">
+        <v>0.9</v>
+      </c>
       <c r="E5" s="2" t="s">
         <v>13</v>
       </c>
@@ -564,149 +572,175 @@
       <c r="C6" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="4"/>
+      <c r="D6" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C7" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="4"/>
+      <c r="D7" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="4"/>
+        <v>12</v>
+      </c>
+      <c r="D8" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="2" t="s">
-        <v>7</v>
+        <v>28</v>
+      </c>
+      <c r="D9" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>30</v>
+      <c r="B10" t="s">
+        <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="4"/>
+        <v>13</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>11</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="4" t="s">
+      <c r="C12" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C12"/>
       <c r="D12" s="4"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>1</v>
-      </c>
       <c r="C13"/>
       <c r="D13" s="4"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="C14"/>
+      <c r="D14" s="4"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D15" s="4"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="D14" s="4"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="B17" s="2"/>
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="D15" s="4"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="B18" s="2"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="2"/>
-      <c r="D16" s="4"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="B19" s="2"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="2"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="B20" s="2"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="2"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="B21" s="2"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="2"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="2"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="B23" s="2"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B21" s="2"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="B24" s="2"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="2"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="B25" s="2"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B26" s="2" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>